<commit_message>
add data dma number
</commit_message>
<xml_diff>
--- a/msg_layer/dolphin_data.xlsx
+++ b/msg_layer/dolphin_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harrywei\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C540FF79-4FC0-4952-9A5C-5DF644BFEB99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DA10BF-F663-4041-844A-0A2B0F423C67}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCIPP" sheetId="1" r:id="rId1"/>
+    <sheet name="DMA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>size</t>
   </si>
@@ -40,6 +41,18 @@
   </si>
   <si>
     <t>x86 to ARM</t>
+  </si>
+  <si>
+    <t>msg size</t>
+  </si>
+  <si>
+    <t>transfer time per msg(us)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X86 to ARM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM to x86 </t>
   </si>
 </sst>
 </file>
@@ -1264,6 +1277,766 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DMA!$C$2:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>X86 to ARM </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>transfer time per msg(us)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DMA!$B$4:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DMA!$C$4:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80.989999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4386-4516-8D8E-46888CB5B39E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="481128608"/>
+        <c:axId val="481136480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="481128608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481136480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="481136480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481128608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DMA!$I$3:$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ARM to x86 </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>transfer time per msg(us)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DMA!$H$5:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DMA!$I$5:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.56</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.71</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.39</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54.53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>108.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8833-47B8-B669-71104B878970}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="281624272"/>
+        <c:axId val="471372408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="281624272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="471372408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="471372408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="281624272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1344,6 +2117,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1861,6 +2714,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2433,6 +4318,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35ABDC2E-9D3E-467A-9148-A786B0547B3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65789ECC-EFCD-4555-82E0-114466B4819F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C91398CC-5F6D-4A7E-A823-5FBD21C7AC72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2718,7 +4680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -3034,4 +4996,255 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A31ED6-A672-4D91-A185-48E7C62ADD90}">
+  <dimension ref="B2:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>128</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="H5" s="1">
+        <v>64</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>256</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H6" s="1">
+        <v>128</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>512</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="H7" s="1">
+        <v>256</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H8" s="1">
+        <v>512</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>2048</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1024</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>4096</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2048</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>8192</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>16384</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.59</v>
+      </c>
+      <c r="H12" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>32768</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.14</v>
+      </c>
+      <c r="H13" s="1">
+        <v>16384</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>65536</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10.25</v>
+      </c>
+      <c r="H14" s="1">
+        <v>32768</v>
+      </c>
+      <c r="I14" s="1">
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>131072</v>
+      </c>
+      <c r="C15" s="1">
+        <v>20.43</v>
+      </c>
+      <c r="H15" s="1">
+        <v>65536</v>
+      </c>
+      <c r="I15" s="1">
+        <v>13.71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>262144</v>
+      </c>
+      <c r="C16" s="1">
+        <v>40.840000000000003</v>
+      </c>
+      <c r="H16" s="1">
+        <v>131072</v>
+      </c>
+      <c r="I16" s="1">
+        <v>27.39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>524288</v>
+      </c>
+      <c r="C17" s="1">
+        <v>80.989999999999995</v>
+      </c>
+      <c r="H17" s="1">
+        <v>262144</v>
+      </c>
+      <c r="I17" s="1">
+        <v>54.53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="1">
+        <v>524288</v>
+      </c>
+      <c r="I18" s="1">
+        <v>108.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>